<commit_message>
3/17/2020 cap winbats, proj plan chg.
</commit_message>
<xml_diff>
--- a/CurrentWork_Delta/JavaScriptFrameDistillationToTheFinish_v1.xlsx
+++ b/CurrentWork_Delta/JavaScriptFrameDistillationToTheFinish_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mark\CurrentWork_Delta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2745FD91-F28A-4557-9876-B8AF1B34D0E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6166FE-0E29-4869-856E-F0D891E0E451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12990" yWindow="-405" windowWidth="12510" windowHeight="17880" xr2:uid="{1C02CC31-4B62-49F7-B75D-EAE54FAFEDF3}"/>
+    <workbookView xWindow="9795" yWindow="870" windowWidth="15570" windowHeight="15105" xr2:uid="{1C02CC31-4B62-49F7-B75D-EAE54FAFEDF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>Expand Unit Test Runs to generate rpt data</t>
   </si>
@@ -167,6 +167,53 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Code Review;  got it.</t>
+  </si>
+  <si>
+    <t>Common.js declarations Figure if there need to go anwhere</t>
+  </si>
+  <si>
+    <t>What else cool stuff did cole put in common.js or move to
+Frame utils…</t>
+  </si>
+  <si>
+    <t>Moved this into third section.  See V3</t>
+  </si>
+  <si>
+    <t>Moved this into Section 2</t>
+  </si>
+  <si>
+    <t>Not doing</t>
+  </si>
+  <si>
+    <t>Moved into the third section</t>
+  </si>
+  <si>
+    <t>completely changed: expanded</t>
+  </si>
+  <si>
+    <t>implemnt rpt frame</t>
+  </si>
+  <si>
+    <t>develop work flow to acces all functions in utils
+Write additional code to generate reporting data</t>
+  </si>
+  <si>
+    <t>Add documentation ( minimally )</t>
+  </si>
+  <si>
+    <t>Minimized the explicit implementation of logging</t>
+  </si>
+  <si>
+    <t>Emphasized implementing log level configuration</t>
+  </si>
+  <si>
+    <t>Apply to all modules</t>
+  </si>
+  <si>
+    <t>Run lots of testing</t>
   </si>
 </sst>
 </file>
@@ -219,9 +266,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -231,11 +275,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,280 +598,348 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCB175D-C41E-43F0-A193-CDB42C3700EA}">
-  <dimension ref="B1:F46"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="53.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="1.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="45.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="1.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>1</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>2</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="2:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="5"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="6"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="1">
         <v>1</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="4" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="1">
         <v>2</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="1" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>